<commit_message>
Add missing talents in Excel file
</commit_message>
<xml_diff>
--- a/WHFRP3.xlsx
+++ b/WHFRP3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\StudioProjects\WarHammerDiceLauncherAndroid\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="0" windowWidth="37060" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="13860" yWindow="0" windowWidth="37065" windowHeight="18375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Talents" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="TYPES_COOLDOWN">Configuration!$D$3:$D$6</definedName>
-    <definedName name="TYPES_TALENT">Configuration!$B$3:$B$8</definedName>
+    <definedName name="TYPES_TALENT">Configuration!$B$3:$B$9</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="229">
   <si>
     <t>Nom</t>
   </si>
@@ -47,9 +52,6 @@
     <t>REPUTATION</t>
   </si>
   <si>
-    <t>FOCUS</t>
-  </si>
-  <si>
     <t>TACTICS</t>
   </si>
   <si>
@@ -450,12 +452,293 @@
   </si>
   <si>
     <t>Vous pouvez dépenser 1 point de fortune lorsque vous êtes affecté par une carte d'état dont la durée est limitée par un nombre de rounds pour réduire cette durée de 2 rounds.</t>
+  </si>
+  <si>
+    <t>Voix de la Raison</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet de substituer votre Intelligence à votre Force Mentale à l'occasion d'un test de compétence. À l'occasion de ce test : {BANE_FACE} Ajoutez {FAILURE_FACE} aux résultats.</t>
+  </si>
+  <si>
+    <t>FAITH</t>
+  </si>
+  <si>
+    <t>Manann, Dieu des Mers</t>
+  </si>
+  <si>
+    <t>Vous bénéficiez d'un {FORTUNE_DICE} à l'occasion de vos tests d'Invocation et de Piété lorsque vous vous trouvez à portée longue ou moins d'une étendue d'eau.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>Morr, Dieu des Rêves et de la Mort</t>
+  </si>
+  <si>
+    <t>Une fois par tour, vous pouvez administrer l'extrême onction de Morr à une personne morte ou mourante qui se trouve à portée courte pour gagner 1 faveur. Ces rites exigent d'effectuer une manœuvre.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>Myrmidia, Déesse de la Guerre</t>
+  </si>
+  <si>
+    <t>Vous gagnez 1 faveur chaque fois que vous obtenez un {SIGMAR_FACE} ou plus lorsque vous portez une Attaque de Corps à Corps.
+Jauge d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Ranald, Dieu de la Chance et de la Tromperie</t>
+  </si>
+  <si>
+    <t>Shallya, Déesse de la Guérison et de la Compassion</t>
+  </si>
+  <si>
+    <t>Chaque fois qu'on de vos alliés qui se trouve à portée courte de vous subit une blessure critique, gagnez 1 faveur.
+Jauge d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Vous commencez chaque session pourvu d'un point de fortune supplémentaire. Lorsque vous dépensez un point de fortune ou plus à l'occasion d'un test de compétence et que ce test est un succès, gagnez 1 faveur.
+Jauge d'Attitude de Départ : PNTTT</t>
+  </si>
+  <si>
+    <t>Sigmar, Dieu de l'Empire</t>
+  </si>
+  <si>
+    <t>Gagnez 1 faveur chaque fois que vous infligez 1 blessure critique ou plus.
+Jauge d'Attitude de Départ : CNTTT</t>
+  </si>
+  <si>
+    <t>Taal, Dieu de la Nature et des Étendues Sauvages</t>
+  </si>
+  <si>
+    <t>Vous bénéficiez d'un {FORTUNE_DICE} à l'occasion de vos tests de Piété et d'Invocation tant que vous vous trouvez en forêt ou dans la nature.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>Ulric, Dieu des Batailles, des Loups et de l'Hiver</t>
+  </si>
+  <si>
+    <t>Gagnez 1 faveur chaque fois que vous subissez une blessure critique.
+Jauge d'Attitude de Départ : PNTTT</t>
+  </si>
+  <si>
+    <t>Verena, Déesse du Savoir et de la Justice</t>
+  </si>
+  <si>
+    <t>Vous pouvez associez un talent Affinité à votre carte de Foi comme si cette dernière était un emplacement de talent de votre fiche de carrière. Tant qu'un talent actif est associé à cet emplacement, vous bénéficiez d'un {FORTUNE_DICE} à l'occasion de vos tests d'Éducation.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>Aqshy, Domaine du Feu, Ordre Flamboyant</t>
+  </si>
+  <si>
+    <t>Lorsque vous infligez des dégâts avec un Sort du Collège Flamboyant, vous pouvez augmenter ces dégâts de 1 pour chaque point d'énergie supplémentaire que vous choisissez d'investir.</t>
+  </si>
+  <si>
+    <t>Azyr, Domaine des Cieux, Ordre Céleste</t>
+  </si>
+  <si>
+    <t>Lorsque vous employez un Sort du Collège Céleste, vous pouvez dépenser 1 énergie supplémentaire pour bénéficier d'un {FORTUNE_DICE} supplémentaire à l'occasion de ce test.
+Jauge d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Chamon, Domaine du Métal, Ordre Doré</t>
+  </si>
+  <si>
+    <t>Lorsque vous employez un Sort de l'Ordre Doré, vous pouvez dépenser 1 énergie pour convertir un de vos dés de caractéristiques {CHARACTERISTIC_DICE} en dé de prudence {CONSERVATIVE_DICE}, quelle que soit votre attitude actuelle.
+Jaude d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Ghur, Domaine des Bêtes, Ordre d'Ambre</t>
+  </si>
+  <si>
+    <t>Tant que vous êtes sous Forme Animale, vous pouvez dépenser 1 énergie pour effectuer une manœuvre supplémentaire lors de votre tour. Il n'est possible de dépenser que 1 énergie de la sorte par tour.
+Jauge d'Attitude de Départ : PNTTT</t>
+  </si>
+  <si>
+    <t>Ghyran, Domaine de la Vie, Ordre de Jade</t>
+  </si>
+  <si>
+    <t>Vous bénéficiez d'un {FORTUNE_DICE} lorsque vous employez un Sort du Collège de Jade si la saison mentionnée par ce sort correspond à la saison actuelle. Si la saison mentionnée est l'opposé de la saison actuelle, vous devez en revanche ajouter un {MISFORTUNE_DICE} à votre réserve de dés.
+Jauge d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Hysh, Domaine de la Lumière, Ordre Lumineux</t>
+  </si>
+  <si>
+    <t>Après avoir lancé un Sort de l'Ordre Lumineux, vous pouvez dépenser 1 énergie afin de retirer ou d'ajouter un jeton de recharge à ce sort ou à une carte d'état obtenue à l'aide de celui-ci.
+Jauge d'Attitude de Départ : PPPNT</t>
+  </si>
+  <si>
+    <t>Magie Noire</t>
+  </si>
+  <si>
+    <t>Vous pouvez apprendre et employer des Sorts de Magie Noire et des Sorts du Chaos. Lorsque vous focalisez l'énergie ou que vous lancez un sort, vous bénéficiez d'un {EXPERTISE_DICE} à l'occasion de votre test. Si vous générez un ou plusieurs {EXERTION_FACE} ou {DELAY_FACE} à l'occasion de ces tests, ajoutez {CHAOS_FACE} aux résultats.
+À l'occasion de vos tests de Focalisation et l'Art de la magie, {BANE_DICE} {BANE_DICE} Ajoutez {CHAOS_FACE} aux résultats.</t>
+  </si>
+  <si>
+    <t>Shyish, Domaine de la Mort, Ordre d'Améthyste</t>
+  </si>
+  <si>
+    <t>Si une créature vivante meurt au cours d'un tour qui suit immédiatement un tour ou vous avez employé un Sort de l'Ordre d'Améthyste, vous pouvez immédiatement dépenser 1 énergie afin d'ajouter ou de retirer 1 jeton de recharge se trouvant sur une de vos cartes d'action de Sort de l'Ordre d'Améthyste.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>Ulgu, Dmaine des Ombres, Ordre Gris</t>
+  </si>
+  <si>
+    <t>Vous pouvez dépenser 1 énergie supplémentaire lorsque vous employez un Sort de l'Ordre Gris afin d'ajouter ou de retirer 1 jeton de recharge à sa carte d'action.
+Jauge d'Attitude de Départ : PPNTT</t>
+  </si>
+  <si>
+    <t>À Bras-le-Corps</t>
+  </si>
+  <si>
+    <t>Si vous êtes engagé au combat avec une cible qui tente d'employer la Défense Active Esquive et que votre Attaque de Corps à Corps réussit malgré tout, rajoutez un jeton de recharge supplémentaire sur sa carte d'action Esquive.</t>
+  </si>
+  <si>
+    <t>Assaut sans Relâche</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet de relancer tous les {FORTUNE_DICE} et les {MISFORTUNE_DICE} suite à un test de Force, d'Endurance ou d'Agilité.</t>
+  </si>
+  <si>
+    <t>Cavalier Invétéré</t>
+  </si>
+  <si>
+    <t>Toutes les attques que vous effectuez alors que vous êtes monté bénéficient d'un {FORTUNE_DICE} supplémentaire. Toutes les formes actives de défense dont vous vous servez alors que vous êtes à cheval imposent un {MISFORTUNE_DICE} supplémentaire aux attaques portées contre vous.</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Vous bénéficiez d'un {FORTUNE_DICE} à l'occasion de toutes vos Attaques de Corps à Corps au cours d'un tour où vous engagez le combat avec un ennemi.</t>
+  </si>
+  <si>
+    <t>Coup de Rein</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet de bénéficier de {FORTUNE_DICE} {FORTUNE_DICE} à l'occasion de n'importe quel test de Force. Si ce test est un échec, gagnez 1 fatigue.</t>
+  </si>
+  <si>
+    <t>Couteau dans la Plaie</t>
+  </si>
+  <si>
+    <t>Vous pouvez infliger 1 fatigue à votre cible en effectuant une manœuvre supplémentaire immédiatement après l'avoir attaquée au corps à corps.</t>
+  </si>
+  <si>
+    <t>Efforts Coordonnés</t>
+  </si>
+  <si>
+    <t>À l'occasion d'un test d'Agilité pour lequel vous avez dépensé des points de fortune, {BOON_FACE} {BOON_FACE} Ajoutez {SUCCESS_FACE} aux résultats.</t>
+  </si>
+  <si>
+    <t>Entraînement Exceptionnel</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet d'annulez jusqu'à {BANE_FACE} {BANE_FACE} lors de vos tests de Force, d'Agilité ou d'Endurance.</t>
+  </si>
+  <si>
+    <t>Escrimeur</t>
+  </si>
+  <si>
+    <t>Votre valeur de défense augmente de 1 lorsque vous êtes armé d'une arme d'escrime ou d'une arme d'escrime et d'une dague.</t>
+  </si>
+  <si>
+    <t>Exploiter les Vulnérabilités</t>
+  </si>
+  <si>
+    <t>Vous bénéficez d'un {FORTUNE_DICE} à l'occasion de vos attaques lorsque votre adversaire souffre d'une blessure critique.</t>
+  </si>
+  <si>
+    <t>Fait de Fer</t>
+  </si>
+  <si>
+    <t>Si vous gagnez 2 points de fatigue ou plus d'un seul coup, ce total est réduit de 1.</t>
+  </si>
+  <si>
+    <t>Impavide</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet d'augmenter votre valeur d'encaissement de 2 contre une source de dégâts. Vous pouvez utiliser ce talent après avoir pris connaissance des dégâts.</t>
+  </si>
+  <si>
+    <t>Intouchable</t>
+  </si>
+  <si>
+    <t>Vous pouvez subir 1 fatigue pour utiliser la défense active Parade contre Attaque à Distance.</t>
+  </si>
+  <si>
+    <t>La Force Justifie Tout</t>
+  </si>
+  <si>
+    <t>À l'occasion d'un test de Force pour lequel vous avez dépensé des points de fortune, {FORTUNE_FACE} {FORTUNE_FACE} Ajoutez {SUCCESS_FACE} aux résultats.</t>
+  </si>
+  <si>
+    <t>Manœuvre sur les Flancs</t>
+  </si>
+  <si>
+    <t>Tant que vous êtes engagé au combat avec au moins 1 allié, vous et vos alliés bénéficiez tous d'un {FORTUNE_DICE} supplémentaire à l'occasion de vos Attaques au Corps à Corps.</t>
+  </si>
+  <si>
+    <t>Meneur au Front</t>
+  </si>
+  <si>
+    <t>Vous bénéficiez d'un {FORTUNE_DICE} à l'occasion d'un test de compétence si aucun ennemi n'a agi depuis le début du tour en cours.</t>
+  </si>
+  <si>
+    <t>Mur de Boucliers</t>
+  </si>
+  <si>
+    <t>Votre valeur de défense augmente de +1 si vous vous battez aux côtés d'au moins deux alliés équipés de boucliers.</t>
+  </si>
+  <si>
+    <t>Pas de Repos pour les Braves</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet d'éliminer 2 fatigue.</t>
+  </si>
+  <si>
+    <t>Poursuite sans Relâche</t>
+  </si>
+  <si>
+    <t>Vous jouissez d'une manœuvre gratuite dès que vous vainquez le dernier ennemi avec lequel vous étiez aux prises.</t>
+  </si>
+  <si>
+    <t>Réflexes Éclairs</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous permet de bénéficier de {FORTUNE_DICE} {FORTUNE_DICE} à l'occasion d'un test d'Agilité ou impose {MISFORTUNE_DICE} {MISFORTUNE_DICE} à une tentative d'Esquive. SI votre test d'Agilité est un échec, gagnez 1 fatigue.</t>
+  </si>
+  <si>
+    <t>Sens du Combat</t>
+  </si>
+  <si>
+    <t>Votre valeur de défense contre les Attaques de Corps à Corps augmente de 1 lorsque aucune de vos cartes d'action Défensive n'est en recharge.</t>
+  </si>
+  <si>
+    <t>Serrer les Dents</t>
+  </si>
+  <si>
+    <t>À l'occasion d'un test d'Endurance pour lequel vous avez dépensé des points de fortune, {BOON_FACE} {BOON_FACE} Ajoutez {SUCCESS_FACE} aux résultats.</t>
+  </si>
+  <si>
+    <t>Robuste</t>
+  </si>
+  <si>
+    <t>Le niveau de gravité de vos blessures critiques est réduit de 1 lorsqu'elles sont traitées ou guéries, jusqu'à un minimum de 1. Les blessures critiques dont le niveau de gravité déjà égal à 0 ne sont pas affectées par ce talent.</t>
+  </si>
+  <si>
+    <t>Vigilance</t>
+  </si>
+  <si>
+    <t>Épuiser cette carte vous confère {FORTUNE_DICE} {FORTUNE_DICE} à l'occasion d'un test d'Initiative.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -575,7 +858,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -602,6 +885,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -624,27 +910,35 @@
       <alignment horizontal="general" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:E66" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="B2:E66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:E108" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B2:E108"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Nom" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Type" dataDxfId="2"/>
-    <tableColumn id="4" name="Cooldown" dataDxfId="1"/>
+    <tableColumn id="1" name="Nom" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" name="Type" dataDxfId="1"/>
+    <tableColumn id="4" name="Cooldown" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -972,23 +1266,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E66"/>
+  <dimension ref="B1:E109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="1" max="1" width="1.125" customWidth="1"/>
+    <col min="2" max="2" width="46.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.5" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="7" customHeight="1"/>
-    <row r="2" spans="2:5">
+    <row r="1" spans="2:5" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1002,910 +1296,1510 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="30">
+    <row r="3" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="30">
-      <c r="B31" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="5" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="30">
-      <c r="B32" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="5" t="s">
+    <row r="45" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="30">
-      <c r="B33" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="5" t="s">
+    <row r="48" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="30">
-      <c r="B34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="5" t="s">
+    <row r="51" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="30">
-      <c r="B35" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="5" t="s">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B54" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B57" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="45">
-      <c r="B36" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="5" t="s">
+    <row r="59" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="30">
-      <c r="B37" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="5" t="s">
+    <row r="65" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B65" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B66" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="30">
-      <c r="B38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="5" t="s">
+    <row r="67" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B72" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B76" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="5" t="s">
+    <row r="87" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="45">
-      <c r="B40" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" s="7" t="s">
+    <row r="90" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="30">
-      <c r="B41" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="5" t="s">
+    <row r="93" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="30">
-      <c r="B42" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" s="5" t="s">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B100" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B101" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="30">
-      <c r="B43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="B44" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="30">
-      <c r="B45" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="8" t="s">
+    <row r="103" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B103" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="30">
-      <c r="B46" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="8" t="s">
+    <row r="104" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="45">
-      <c r="B47" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="30">
-      <c r="B48" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="8" t="s">
+    <row r="105" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="45">
-      <c r="B51" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="30">
-      <c r="B52" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5">
-      <c r="B53" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="30">
-      <c r="B54" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="30">
-      <c r="B55" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="45">
-      <c r="B56" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="45">
-      <c r="B57" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="30">
-      <c r="B58" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="30">
-      <c r="B59" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="30">
-      <c r="B60" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="45">
-      <c r="B62" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="30">
-      <c r="B63" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5">
-      <c r="B64" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="30">
-      <c r="B65" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5">
-      <c r="B66" s="11">
-        <v>5.2083333333333336E-2</v>
-      </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D66">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D108">
       <formula1>TYPES_TALENT</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E66">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E108">
       <formula1>TYPES_COOLDOWN</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -1917,69 +2811,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.125" customWidth="1"/>
+    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.125" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="7" customHeight="1"/>
-    <row r="2" spans="2:4">
+    <row r="1" spans="2:4" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>